<commit_message>
callback 종류 익히기, callback hell 체험
</commit_message>
<xml_diff>
--- a/커리큘럼/식초님 로드맵 정리.xlsx
+++ b/커리큘럼/식초님 로드맵 정리.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\frontEnd_notes\커리큘럼\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C19228A-A34C-436D-A83F-F1E91D261E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770853E4-CFC2-4F53-A5BE-79DAE1F0B592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="2580" windowWidth="21600" windowHeight="11460" xr2:uid="{6A2E78A4-70C6-4F8F-8733-6D8FB6A7E8A2}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="132">
   <si>
     <r>
       <t xml:space="preserve">프론트엔드 공부 순서, 높은 연봉 받는 프론트엔드 개발자 되기 | 해외 개발자 선배가 알려드려요 </t>
@@ -1359,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D3A1F8-0818-4133-A35C-33D74C6F4A48}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2002,7 +2002,9 @@
       <c r="C37" s="26">
         <v>0.88611111111111107</v>
       </c>
-      <c r="D37" s="50"/>
+      <c r="D37" s="50" t="s">
+        <v>100</v>
+      </c>
       <c r="E37" s="61" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
Revert "callback 종류 익히기, callback hell 체험"
This reverts commit fe5761264e3d6d40c8af4c1d180b27a35d0911f9.
</commit_message>
<xml_diff>
--- a/커리큘럼/식초님 로드맵 정리.xlsx
+++ b/커리큘럼/식초님 로드맵 정리.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\frontEnd_notes\커리큘럼\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770853E4-CFC2-4F53-A5BE-79DAE1F0B592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C19228A-A34C-436D-A83F-F1E91D261E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="2580" windowWidth="21600" windowHeight="11460" xr2:uid="{6A2E78A4-70C6-4F8F-8733-6D8FB6A7E8A2}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="132">
   <si>
     <r>
       <t xml:space="preserve">프론트엔드 공부 순서, 높은 연봉 받는 프론트엔드 개발자 되기 | 해외 개발자 선배가 알려드려요 </t>
@@ -1359,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D3A1F8-0818-4133-A35C-33D74C6F4A48}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2002,9 +2002,7 @@
       <c r="C37" s="26">
         <v>0.88611111111111107</v>
       </c>
-      <c r="D37" s="50" t="s">
-        <v>100</v>
-      </c>
+      <c r="D37" s="50"/>
       <c r="E37" s="61" t="s">
         <v>127</v>
       </c>

</xml_diff>